<commit_message>
auth.json file added instead of login again and again
</commit_message>
<xml_diff>
--- a/data/ouput/InstaLeaderShip.xlsx
+++ b/data/ouput/InstaLeaderShip.xlsx
@@ -1256,7 +1256,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I154"/>
+  <dimension ref="A1:I156"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A133" workbookViewId="0">
       <selection activeCell="G134" sqref="G134"/>
@@ -8923,28 +8923,28 @@
       </c>
     </row>
     <row r="154">
-      <c r="A154" t="inlineStr">
+      <c r="A154" s="0" t="inlineStr">
         <is>
           <t>Melody McCloskey</t>
         </is>
       </c>
-      <c r="B154" t="inlineStr">
+      <c r="B154" s="0" t="inlineStr">
         <is>
           <t>https://www.instagram.com/melody/</t>
         </is>
       </c>
-      <c r="C154" t="n">
+      <c r="C154" s="0" t="n">
         <v>1503</v>
       </c>
-      <c r="D154" t="n">
+      <c r="D154" s="0" t="n">
         <v>66800</v>
       </c>
-      <c r="E154" t="n">
+      <c r="E154" s="0" t="n">
         <v>903</v>
       </c>
-      <c r="F154" t="inlineStr"/>
-      <c r="G154" t="inlineStr"/>
-      <c r="H154" t="inlineStr">
+      <c r="F154" s="0" t="inlineStr"/>
+      <c r="G154" s="0" t="inlineStr"/>
+      <c r="H154" s="0" t="inlineStr">
         <is>
           <t>Melody McCloskey
 melody
@@ -8953,7 +8953,7 @@
 more</t>
         </is>
       </c>
-      <c r="I154" t="inlineStr">
+      <c r="I154" s="0" t="inlineStr">
         <is>
           <t>melody
 Follow
@@ -8969,6 +8969,130 @@
         </is>
       </c>
     </row>
+    <row r="155">
+      <c r="A155" s="0" t="inlineStr">
+        <is>
+          <t>Arian Hushyar Van de Carr</t>
+        </is>
+      </c>
+      <c r="B155" s="0" t="inlineStr">
+        <is>
+          <t>https://www.instagram.com/arianvdc/</t>
+        </is>
+      </c>
+      <c r="C155" s="0" t="n">
+        <v>960</v>
+      </c>
+      <c r="D155" s="0" t="n">
+        <v>460</v>
+      </c>
+      <c r="E155" s="0" t="n">
+        <v>1493</v>
+      </c>
+      <c r="F155" s="0" t="inlineStr"/>
+      <c r="G155" s="0" t="inlineStr">
+        <is>
+          <t>supplefi.co</t>
+        </is>
+      </c>
+      <c r="H155" s="0" t="inlineStr">
+        <is>
+          <t>Arian Hushyar Van de Carr
+arianvdc
+🌟 Jesus
+✨ Co-founder &amp; CEO @supplefi_official
+🏡 livin’ in Austin
+❤️ married to @kedricv
+👦🏻 👧🏻 👦🏻 my babies: Knox,... 
+more
+supplefi.co</t>
+        </is>
+      </c>
+      <c r="I155" s="0" t="inlineStr">
+        <is>
+          <t>arianvdc
+Follow
+960 posts
+460 followers
+1,493 following
+Arian Hushyar Van de Carr
+arianvdc
+🌟 Jesus
+✨ Co-founder &amp; CEO @supplefi_official
+🏡 livin’ in Austin
+❤️ married to @kedricv
+👦🏻 👧🏻 👦🏻 my babies: Knox,... 
+more
+supplefi.co
+My 40th
+Health &amp; Fitnes
+My babies
+Maui</t>
+        </is>
+      </c>
+    </row>
+    <row r="156">
+      <c r="A156" t="inlineStr">
+        <is>
+          <t>Steve Martocci</t>
+        </is>
+      </c>
+      <c r="B156" t="inlineStr">
+        <is>
+          <t>https://www.instagram.com/smart/</t>
+        </is>
+      </c>
+      <c r="C156" t="n">
+        <v>463</v>
+      </c>
+      <c r="D156" t="n">
+        <v>27100</v>
+      </c>
+      <c r="E156" t="n">
+        <v>1745</v>
+      </c>
+      <c r="F156" t="inlineStr"/>
+      <c r="G156" t="inlineStr">
+        <is>
+          <t>supp.co/about/founder-story</t>
+        </is>
+      </c>
+      <c r="H156" t="inlineStr">
+        <is>
+          <t>Steve Martocci
+smart
+Co-Founder of @joinsuppco, @splice , @flyblade &amp; @groupme. Mostly Harmless.
+supp.co/about/founder-story</t>
+        </is>
+      </c>
+      <c r="I156" t="inlineStr">
+        <is>
+          <t>smart
+Follow
+463 posts
+27.1K followers
+1,745 following
+Steve Martocci
+smart
+Co-Founder of @joinsuppco, @splice , @flyblade &amp; @groupme. Mostly Harmless.
+supp.co/about/founder-story
+Porto Marina
+Palisades Fire
+SuppCo
+Jaxson
+Steve 4.0
+Christina
+Cal
+Splice
+Komet
+Christmas '20
+Summer Tour ‘20
+The Phish
+Thanksgiving 19
+Halloween '19</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="G143" display="www.teachaapi.org" r:id="rId1"/>

</xml_diff>